<commit_message>
Ice Spike and lightning base spell speed
</commit_message>
<xml_diff>
--- a/Assets/Systems.xlsx
+++ b/Assets/Systems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project_Witch_Hunt\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C5A0AD-7B74-4399-8666-DAAADF98A2DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126FE297-8CCA-4B50-925C-E1934A258BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{532FCD95-2C2A-4B56-85A4-F5F3E8F1C2DC}"/>
   </bookViews>
@@ -666,15 +666,15 @@
         <v>5</v>
       </c>
       <c r="J5">
-        <f>$I5*(1-J$4)</f>
+        <f t="shared" ref="J5:L7" si="0">$I5*(1-J$4)</f>
         <v>4.5</v>
       </c>
       <c r="K5">
-        <f>$I5*(1-K$4)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L5">
-        <f>$I5*(1-L$4)</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
       <c r="N5" t="s">
@@ -685,15 +685,15 @@
         <v>5</v>
       </c>
       <c r="P5">
-        <f t="shared" ref="P5:R5" si="0">$D3/J5</f>
+        <f t="shared" ref="P5:R5" si="1">$D3/J5</f>
         <v>5.5555555555555554</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.25</v>
       </c>
       <c r="R5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.1428571428571432</v>
       </c>
     </row>
@@ -722,34 +722,34 @@
         <v>7</v>
       </c>
       <c r="J6">
-        <f>$I6*(1-J$4)</f>
+        <f t="shared" si="0"/>
         <v>6.3</v>
       </c>
       <c r="K6">
-        <f>$I6*(1-K$4)</f>
+        <f t="shared" si="0"/>
         <v>5.6000000000000005</v>
       </c>
       <c r="L6">
-        <f>$I6*(1-L$4)</f>
+        <f t="shared" si="0"/>
         <v>4.8999999999999995</v>
       </c>
       <c r="N6" t="s">
         <v>35</v>
       </c>
       <c r="O6">
-        <f t="shared" ref="O6:R6" si="1">$D4/I6</f>
+        <f t="shared" ref="O6:R6" si="2">$D4/I6</f>
         <v>5</v>
       </c>
       <c r="P6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.5555555555555554</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.2499999999999991</v>
       </c>
       <c r="R6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.1428571428571432</v>
       </c>
     </row>
@@ -774,34 +774,34 @@
         <v>12</v>
       </c>
       <c r="J7">
-        <f>$I7*(1-J$4)</f>
+        <f t="shared" si="0"/>
         <v>10.8</v>
       </c>
       <c r="K7">
-        <f>$I7*(1-K$4)</f>
+        <f t="shared" si="0"/>
         <v>9.6000000000000014</v>
       </c>
       <c r="L7">
-        <f>$I7*(1-L$4)</f>
+        <f t="shared" si="0"/>
         <v>8.3999999999999986</v>
       </c>
       <c r="N7" t="s">
         <v>36</v>
       </c>
       <c r="O7">
-        <f t="shared" ref="O7:R7" si="2">$D5/I7</f>
+        <f t="shared" ref="O7:R7" si="3">$D5/I7</f>
         <v>5</v>
       </c>
       <c r="P7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.5555555555555554</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.2499999999999991</v>
       </c>
       <c r="R7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.1428571428571441</v>
       </c>
     </row>
@@ -826,15 +826,15 @@
         <v>7.5</v>
       </c>
       <c r="P8">
-        <f t="shared" ref="P8:R8" si="3">$D6/J7</f>
+        <f t="shared" ref="P8:R8" si="4">$D6/J7</f>
         <v>8.3333333333333321</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.3749999999999982</v>
       </c>
       <c r="R8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10.714285714285715</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Particles on status | Special Spell UI | Fix Enemy Death Behavior
</commit_message>
<xml_diff>
--- a/Assets/Systems.xlsx
+++ b/Assets/Systems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project_Witch_Hunt\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDBEA4A-1C98-443C-A0C7-D43467C7CFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41831193-5A2C-4B4C-A8AF-C93BE32E048C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{532FCD95-2C2A-4B56-85A4-F5F3E8F1C2DC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{532FCD95-2C2A-4B56-85A4-F5F3E8F1C2DC}"/>
   </bookViews>
   <sheets>
     <sheet name="CharacterStats" sheetId="3" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">SpecialSpellsStats!$A$1:$M$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="79">
   <si>
     <t>Base Spells</t>
   </si>
@@ -277,6 +278,9 @@
   </si>
   <si>
     <t>Dmg/Sec goal</t>
+  </si>
+  <si>
+    <t>{TotTotalDamg</t>
   </si>
 </sst>
 </file>
@@ -285,7 +289,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -328,11 +332,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,26 +674,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A50200A-D5C9-4036-ACBE-BAEB92E92EFD}">
   <dimension ref="A2:W45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="J43" sqref="J43:J45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>29</v>
       </c>
@@ -700,7 +704,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -717,23 +721,23 @@
       <c r="G3">
         <v>7</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="O3" s="3" t="s">
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="O3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
       <c r="W3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -784,12 +788,12 @@
       <c r="V4" t="s">
         <v>6</v>
       </c>
-      <c r="W4" s="4">
+      <c r="W4" s="3">
         <f>BaseSpellsStats!E2/BaseSpellsStats!F2</f>
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -830,11 +834,11 @@
         <v>33</v>
       </c>
       <c r="O5">
-        <f>$D3/I5</f>
+        <f t="shared" ref="O5:R7" si="1">$D3/I5</f>
         <v>17.5</v>
       </c>
       <c r="P5">
-        <f t="shared" ref="P5:R5" si="1">$D3/J5</f>
+        <f t="shared" si="1"/>
         <v>19.444444444444443</v>
       </c>
       <c r="Q5">
@@ -851,12 +855,12 @@
       <c r="V5" t="s">
         <v>7</v>
       </c>
-      <c r="W5" s="4">
+      <c r="W5" s="3">
         <f>BaseSpellsStats!E3/BaseSpellsStats!F3</f>
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -897,19 +901,19 @@
         <v>34</v>
       </c>
       <c r="O6">
-        <f t="shared" ref="O6:R6" si="2">$D4/I6</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="P6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>18.888888888888889</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>21.249999999999996</v>
       </c>
       <c r="R6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>24.285714285714288</v>
       </c>
       <c r="U6" t="s">
@@ -918,12 +922,12 @@
       <c r="V6" t="s">
         <v>8</v>
       </c>
-      <c r="W6" s="4">
+      <c r="W6" s="3">
         <f>BaseSpellsStats!E4/BaseSpellsStats!F4</f>
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -959,19 +963,19 @@
         <v>35</v>
       </c>
       <c r="O7">
-        <f t="shared" ref="O7:R7" si="3">$D5/I7</f>
+        <f t="shared" si="1"/>
         <v>14.291666666666666</v>
       </c>
       <c r="P7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>15.879629629629628</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>17.864583333333332</v>
       </c>
       <c r="R7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>20.416666666666671</v>
       </c>
       <c r="U7" t="s">
@@ -980,12 +984,12 @@
       <c r="V7" t="s">
         <v>6</v>
       </c>
-      <c r="W7" s="4">
+      <c r="W7" s="3">
         <f>BaseSpellsStats!E5/BaseSpellsStats!F5</f>
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1011,15 +1015,15 @@
         <v>18.579166666666669</v>
       </c>
       <c r="P8">
-        <f t="shared" ref="P8:R8" si="4">$D6/J7</f>
+        <f>$D6/J7</f>
         <v>20.643518518518519</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="4"/>
+        <f>$D6/K7</f>
         <v>23.223958333333332</v>
       </c>
       <c r="R8">
-        <f t="shared" si="4"/>
+        <f>$D6/L7</f>
         <v>26.541666666666675</v>
       </c>
       <c r="U8" t="s">
@@ -1028,12 +1032,12 @@
       <c r="V8" t="s">
         <v>7</v>
       </c>
-      <c r="W8" s="4">
+      <c r="W8" s="3">
         <f>BaseSpellsStats!E6/BaseSpellsStats!F6</f>
         <v>16.666666666666668</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1060,12 +1064,12 @@
       <c r="V9" t="s">
         <v>8</v>
       </c>
-      <c r="W9" s="4">
+      <c r="W9" s="3">
         <f>BaseSpellsStats!E7/BaseSpellsStats!F7</f>
         <v>26.666666666666668</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1092,12 +1096,12 @@
       <c r="V10" t="s">
         <v>6</v>
       </c>
-      <c r="W10" s="4">
+      <c r="W10" s="3">
         <f>BaseSpellsStats!E8/BaseSpellsStats!F8</f>
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1116,12 +1120,12 @@
       <c r="V11" t="s">
         <v>7</v>
       </c>
-      <c r="W11" s="4">
+      <c r="W11" s="3">
         <f>BaseSpellsStats!E9/BaseSpellsStats!F9</f>
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1140,12 +1144,12 @@
       <c r="V12" t="s">
         <v>8</v>
       </c>
-      <c r="W12" s="4">
+      <c r="W12" s="3">
         <f>BaseSpellsStats!E10/BaseSpellsStats!F10</f>
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1159,7 +1163,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1175,12 +1179,12 @@
       <c r="V14" t="s">
         <v>6</v>
       </c>
-      <c r="W14" s="4">
+      <c r="W14" s="3">
         <f>AVERAGE(W10, W7, W4)</f>
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1200,12 +1204,12 @@
       <c r="V15" t="s">
         <v>7</v>
       </c>
-      <c r="W15" s="4">
+      <c r="W15" s="3">
         <f>AVERAGE(W11, W8, W5)</f>
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1225,12 +1229,12 @@
       <c r="V16" t="s">
         <v>8</v>
       </c>
-      <c r="W16" s="4">
+      <c r="W16" s="3">
         <f>AVERAGE(W12, W9, W6)</f>
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1245,7 +1249,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1264,12 +1268,12 @@
       <c r="V18" t="s">
         <v>6</v>
       </c>
-      <c r="W18" s="4">
+      <c r="W18" s="3">
         <f>BaseSpellsStats!E11/BaseSpellsStats!F11</f>
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1292,12 +1296,12 @@
       <c r="V19" t="s">
         <v>7</v>
       </c>
-      <c r="W19" s="4">
+      <c r="W19" s="3">
         <f>BaseSpellsStats!E12/BaseSpellsStats!F12</f>
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1320,12 +1324,12 @@
       <c r="V20" t="s">
         <v>8</v>
       </c>
-      <c r="W20" s="4">
+      <c r="W20" s="3">
         <f>BaseSpellsStats!E13/BaseSpellsStats!F13</f>
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1352,7 +1356,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="U22" t="s">
         <v>57</v>
       </c>
@@ -1363,7 +1367,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="U23" t="s">
         <v>57</v>
       </c>
@@ -1374,39 +1378,39 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V25" t="s">
         <v>6</v>
       </c>
-      <c r="W25" s="4">
+      <c r="W25" s="3">
         <f>AVERAGE(W18,W21)</f>
         <v>12.5</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V26" t="s">
         <v>7</v>
       </c>
-      <c r="W26" s="4">
+      <c r="W26" s="3">
         <f>AVERAGE(W19,W22)</f>
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V27" t="s">
         <v>8</v>
       </c>
-      <c r="W27" s="4">
+      <c r="W27" s="3">
         <f>AVERAGE(W20,W23)</f>
         <v>24.5</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F33" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>57</v>
       </c>
@@ -1416,7 +1420,7 @@
       <c r="C34" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="3">
         <f>W14*F34</f>
         <v>32</v>
       </c>
@@ -1424,7 +1428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>57</v>
       </c>
@@ -1434,7 +1438,7 @@
       <c r="C35" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="3">
         <f>W15*F35</f>
         <v>84.444444444444443</v>
       </c>
@@ -1442,7 +1446,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>57</v>
       </c>
@@ -1452,7 +1456,7 @@
       <c r="C36" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="3">
         <f>W16*F36</f>
         <v>161.33333333333334</v>
       </c>
@@ -1460,7 +1464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>58</v>
       </c>
@@ -1470,7 +1474,7 @@
       <c r="C37" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="3">
         <f>W14*F37</f>
         <v>42.666666666666664</v>
       </c>
@@ -1478,7 +1482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -1488,7 +1492,7 @@
       <c r="C38" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D38" s="3">
         <f>W15*F38</f>
         <v>101.33333333333334</v>
       </c>
@@ -1496,7 +1500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>58</v>
       </c>
@@ -1506,7 +1510,7 @@
       <c r="C39" t="s">
         <v>8</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D39" s="3">
         <f>W16*F39</f>
         <v>188.22222222222223</v>
       </c>
@@ -1514,7 +1518,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>61</v>
       </c>
@@ -1537,7 +1541,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -1571,7 +1575,7 @@
         <v>8.5714285714285712</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -1605,7 +1609,7 @@
         <v>18.743801652892561</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -1652,23 +1656,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE9C9E1-2B79-4D72-8AA7-2483BAC6B7DE}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1694,7 +1698,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1720,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1746,7 +1750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1772,7 +1776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1798,7 +1802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1824,7 +1828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1850,7 +1854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1876,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1902,7 +1906,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1928,7 +1932,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1949,7 +1953,7 @@
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1970,7 +1974,7 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2050,31 +2054,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F44E55-3490-4989-BF47-DCCD22AFF76E}">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" customWidth="1"/>
+    <col min="16" max="16" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2115,13 +2121,16 @@
         <v>4</v>
       </c>
       <c r="N1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" t="s">
         <v>75</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2135,16 +2144,16 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F2">
         <v>0.8</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2">
         <v>5</v>
@@ -2152,15 +2161,22 @@
       <c r="L2">
         <v>3</v>
       </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
       <c r="N2">
-        <f>D2/E2+H2*F2</f>
-        <v>12</v>
-      </c>
-      <c r="O2" s="5">
+        <f>D2+F2*G2*H2</f>
+        <v>51.2</v>
+      </c>
+      <c r="O2">
+        <f>N2/E2</f>
+        <v>8.5333333333333332</v>
+      </c>
+      <c r="P2" s="4">
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2174,13 +2190,13 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H3">
         <v>22</v>
@@ -2191,15 +2207,22 @@
       <c r="L3">
         <v>3</v>
       </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
       <c r="N3">
-        <f>D3/E3+H3*F3</f>
-        <v>22</v>
-      </c>
-      <c r="O3" s="5">
+        <f t="shared" ref="N3:N28" si="0">D3+F3*G3*H3</f>
+        <v>79.2</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O28" si="1">N3/E3</f>
+        <v>13.200000000000001</v>
+      </c>
+      <c r="P3" s="4">
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2213,16 +2236,16 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H4">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J4">
         <v>10</v>
@@ -2230,15 +2253,22 @@
       <c r="L4">
         <v>3</v>
       </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
       <c r="N4">
-        <f>D4/E4+H4*F4</f>
-        <v>30</v>
-      </c>
-      <c r="O4" s="5">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="1"/>
+        <v>22.5</v>
+      </c>
+      <c r="P4" s="4">
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2249,10 +2279,10 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F5">
         <v>0.3</v>
@@ -2275,15 +2305,22 @@
       <c r="L5">
         <v>0.1</v>
       </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
       <c r="N5">
-        <f>D5/E5+H5/G5*F5</f>
-        <v>1.5</v>
-      </c>
-      <c r="O5" s="5">
+        <f t="shared" si="0"/>
+        <v>64.5</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="1"/>
+        <v>12.9</v>
+      </c>
+      <c r="P5" s="4">
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2293,24 +2330,49 @@
       <c r="C6">
         <v>2</v>
       </c>
+      <c r="D6">
+        <v>80</v>
+      </c>
       <c r="E6">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>0.5</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
       </c>
       <c r="I6">
         <v>10</v>
       </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
       <c r="L6">
         <v>0.1</v>
       </c>
-      <c r="N6" t="e">
-        <f>D6/E6+H6/G6*F6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O6" s="5">
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="1"/>
+        <v>21.875</v>
+      </c>
+      <c r="P6" s="4">
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2320,24 +2382,49 @@
       <c r="C7">
         <v>3</v>
       </c>
+      <c r="D7">
+        <v>120</v>
+      </c>
       <c r="E7">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
       </c>
       <c r="I7">
         <v>15</v>
       </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
       <c r="L7">
         <v>0.1</v>
       </c>
-      <c r="N7" t="e">
-        <f>D7/E7+H7/G7*F7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O7" s="5">
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>127.5</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="1"/>
+        <v>31.875</v>
+      </c>
+      <c r="P7" s="4">
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -2347,15 +2434,43 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="N8" t="e">
-        <f>D8/E8+H8/G8*F8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O8" s="5">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>0.8</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>25</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="1"/>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="P8" s="4">
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2365,15 +2480,43 @@
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="N9" t="e">
-        <f>D9/E9+H9/G9*F9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O9" s="5">
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>30</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="P9" s="4">
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -2383,15 +2526,43 @@
       <c r="C10">
         <v>3</v>
       </c>
-      <c r="N10" t="e">
-        <f>D10/E10+H10/G10*F10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O10" s="5">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>35</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>3</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="1"/>
+        <v>29.166666666666668</v>
+      </c>
+      <c r="P10" s="4">
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -2401,15 +2572,19 @@
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="N11" t="e">
-        <f>D11/E11+H11/G11*F11</f>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O11" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O11" s="5">
+      <c r="P11" s="4">
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -2419,15 +2594,19 @@
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="N12" t="e">
-        <f>D12/E12+H12/G12*F12</f>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O12" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O12" s="5">
+      <c r="P12" s="4">
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -2437,15 +2616,19 @@
       <c r="C13">
         <v>3</v>
       </c>
-      <c r="N13" t="e">
-        <f>D13/E13+H13/G13*F13</f>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O13" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O13" s="5">
+      <c r="P13" s="4">
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -2455,15 +2638,19 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="N14" t="e">
-        <f>D14/E14+H14/G14*F14</f>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O14" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O14" s="5">
+      <c r="P14" s="4">
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -2473,15 +2660,19 @@
       <c r="C15">
         <v>2</v>
       </c>
-      <c r="N15" t="e">
-        <f>D15/E15+H15/G15*F15</f>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O15" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O15" s="5">
+      <c r="P15" s="4">
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -2491,15 +2682,19 @@
       <c r="C16">
         <v>3</v>
       </c>
-      <c r="N16" t="e">
-        <f>D16/E16+H16/G16*F16</f>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O16" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O16" s="5">
+      <c r="P16" s="4">
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -2509,15 +2704,19 @@
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="N17" t="e">
-        <f>D17/E17+H17/G17*F17</f>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O17" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O17" s="5">
+      <c r="P17" s="4">
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -2527,15 +2726,19 @@
       <c r="C18">
         <v>2</v>
       </c>
-      <c r="N18" t="e">
-        <f>D18/E18+H18/G18*F18</f>
+      <c r="N18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O18" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O18" s="5">
+      <c r="P18" s="4">
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -2545,15 +2748,19 @@
       <c r="C19">
         <v>3</v>
       </c>
-      <c r="N19" t="e">
-        <f>D19/E19+H19/G19*F19</f>
+      <c r="N19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O19" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O19" s="5">
+      <c r="P19" s="4">
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -2563,15 +2770,19 @@
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="N20" t="e">
-        <f>D20/E20+H20/G20*F20</f>
+      <c r="N20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O20" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O20" s="5">
+      <c r="P20" s="4">
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -2581,15 +2792,19 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="N21" t="e">
-        <f>D21/E21+H21/G21*F21</f>
+      <c r="N21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O21" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O21" s="5">
+      <c r="P21" s="4">
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2599,15 +2814,19 @@
       <c r="C22">
         <v>3</v>
       </c>
-      <c r="N22" t="e">
-        <f>D22/E22+H22/G22*F22</f>
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O22" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O22" s="5">
+      <c r="P22" s="4">
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -2617,15 +2836,19 @@
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="N23" t="e">
-        <f>D23/E23+H23/G23*F23</f>
+      <c r="N23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O23" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O23" s="5">
+      <c r="P23" s="4">
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -2635,15 +2858,19 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="N24" t="e">
-        <f>D24/E24+H24/G24*F24</f>
+      <c r="N24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O24" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O24" s="5">
+      <c r="P24" s="4">
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -2653,15 +2880,19 @@
       <c r="C25">
         <v>3</v>
       </c>
-      <c r="N25" t="e">
-        <f>D25/E25+H25/G25*F25</f>
+      <c r="N25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O25" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O25" s="5">
+      <c r="P25" s="4">
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -2671,15 +2902,19 @@
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="N26" t="e">
-        <f>D26/E26+H26/G26*F26</f>
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O26" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O26" s="5">
+      <c r="P26" s="4">
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -2689,15 +2924,19 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="N27" t="e">
-        <f>D27/E27+H27/G27*F27</f>
+      <c r="N27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O27" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O27" s="5">
+      <c r="P27" s="4">
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -2707,11 +2946,15 @@
       <c r="C28">
         <v>3</v>
       </c>
-      <c r="N28" t="e">
-        <f>D28/E28+H28/G28*F28</f>
+      <c r="N28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O28" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O28" s="5">
+      <c r="P28" s="4">
         <v>26.888888888888889</v>
       </c>
     </row>
@@ -2728,13 +2971,13 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="125.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="125.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2748,7 +2991,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2762,7 +3005,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2776,7 +3019,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2790,7 +3033,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2804,7 +3047,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2818,7 +3061,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2832,7 +3075,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2846,7 +3089,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -2860,7 +3103,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -2874,7 +3117,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -2888,7 +3131,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -2902,7 +3145,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Spell Numbers and SriptObj
</commit_message>
<xml_diff>
--- a/Assets/Systems.xlsx
+++ b/Assets/Systems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project_Witch_Hunt\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41831193-5A2C-4B4C-A8AF-C93BE32E048C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098FBA9B-C377-4BD3-B1E2-577DA27FC36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{532FCD95-2C2A-4B56-85A4-F5F3E8F1C2DC}"/>
   </bookViews>
@@ -19,11 +19,10 @@
     <sheet name="Dictionary" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BaseSpellsStats!$A$1:$H$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">SpecialSpellsStats!$A$1:$M$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BaseSpellsStats!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">SpecialSpellsStats!$A$1:$Q$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="83">
   <si>
     <t>Base Spells</t>
   </si>
@@ -281,6 +280,18 @@
   </si>
   <si>
     <t>{TotTotalDamg</t>
+  </si>
+  <si>
+    <t>Rate Of Fire (shots/sec)</t>
+  </si>
+  <si>
+    <t>TotalDmg</t>
+  </si>
+  <si>
+    <t>TotalDmg/sec</t>
+  </si>
+  <si>
+    <t>StatusEffect Dmg</t>
   </si>
 </sst>
 </file>
@@ -307,12 +318,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -328,7 +351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -337,6 +360,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A50200A-D5C9-4036-ACBE-BAEB92E92EFD}">
   <dimension ref="A2:W45"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43:J45"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1138,6 +1163,9 @@
       <c r="D12" s="2">
         <v>0.1</v>
       </c>
+      <c r="E12">
+        <v>180</v>
+      </c>
       <c r="U12" t="s">
         <v>3</v>
       </c>
@@ -1162,6 +1190,9 @@
       <c r="D13" s="2">
         <v>0.2</v>
       </c>
+      <c r="E13">
+        <v>2363</v>
+      </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1175,6 +1206,9 @@
       </c>
       <c r="D14" s="2">
         <v>0.3</v>
+      </c>
+      <c r="E14">
+        <v>6863</v>
       </c>
       <c r="V14" t="s">
         <v>6</v>
@@ -1654,10 +1688,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE9C9E1-2B79-4D72-8AA7-2483BAC6B7DE}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1668,11 +1702,12 @@
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1692,13 +1727,22 @@
         <v>11</v>
       </c>
       <c r="G1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1717,14 +1761,25 @@
       <c r="F2">
         <v>0.5</v>
       </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f>E2+G2*H2*I2</f>
+        <v>6</v>
+      </c>
+      <c r="K2">
+        <f>J2/F2</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1743,14 +1798,25 @@
       <c r="F3">
         <v>0.5</v>
       </c>
-      <c r="G3" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <f>E3+G3*H3*I3</f>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="K3">
+        <f>J3/F3</f>
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1769,14 +1835,25 @@
       <c r="F4">
         <v>0.5</v>
       </c>
-      <c r="G4" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="H4">
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="I4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <f>E4+G4*H4*I4</f>
+        <v>15.5</v>
+      </c>
+      <c r="K4">
+        <f>J4/F4</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1795,14 +1872,22 @@
       <c r="F5">
         <v>0.3</v>
       </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f>E5+G5</f>
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <f>J5/F5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1821,14 +1906,22 @@
       <c r="F6">
         <v>0.3</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>0.3</v>
       </c>
-      <c r="H6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <f>E6+G6</f>
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <f>J6/F6</f>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1847,14 +1940,22 @@
       <c r="F7">
         <v>0.3</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>0.5</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <f>E7+G7</f>
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <f>J7/F7</f>
+        <v>26.666666666666668</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1873,14 +1974,22 @@
       <c r="F8">
         <v>0.5</v>
       </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f>E8+G8</f>
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <f>J8/F8</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1899,14 +2008,22 @@
       <c r="F9">
         <v>0.5</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>0.3</v>
       </c>
-      <c r="H9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <f>E9+G9</f>
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <f>J9/F9</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1925,14 +2042,22 @@
       <c r="F10">
         <v>0.5</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>0.5</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <f>E10+G10</f>
+        <v>13</v>
+      </c>
+      <c r="K10">
+        <f>J10/F10</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1951,9 +2076,9 @@
       <c r="F11">
         <v>0.5</v>
       </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1972,9 +2097,9 @@
       <c r="F12">
         <v>0.5</v>
       </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1993,10 +2118,10 @@
       <c r="F13">
         <v>0.5</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{8FE9C9E1-2B79-4D72-8AA7-2483BAC6B7DE}"/>
+  <autoFilter ref="A1:I1" xr:uid="{8FE9C9E1-2B79-4D72-8AA7-2483BAC6B7DE}"/>
   <conditionalFormatting sqref="C2:C13">
     <cfRule type="colorScale" priority="7">
       <colorScale>
@@ -2033,7 +2158,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F13">
+  <conditionalFormatting sqref="F2:G13">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2054,10 +2179,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F44E55-3490-4989-BF47-DCCD22AFF76E}">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2067,20 +2192,21 @@
     <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5546875" customWidth="1"/>
-    <col min="16" max="16" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" customWidth="1"/>
+    <col min="17" max="17" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2097,13 +2223,13 @@
         <v>11</v>
       </c>
       <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
         <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>76</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -2121,16 +2247,19 @@
         <v>4</v>
       </c>
       <c r="N1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" t="s">
         <v>78</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>75</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2147,36 +2276,42 @@
         <v>6</v>
       </c>
       <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>18</v>
+      </c>
+      <c r="H2">
         <v>0.8</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>16</v>
       </c>
       <c r="J2">
         <v>5</v>
       </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
       <c r="L2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <f>D2+F2*G2*H2</f>
-        <v>51.2</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <f>N2/E2</f>
-        <v>8.5333333333333332</v>
-      </c>
-      <c r="P2" s="4">
+        <f>D2+(G2*H2*F2)</f>
+        <v>57.6</v>
+      </c>
+      <c r="P2">
+        <f>O2/E2</f>
+        <v>9.6</v>
+      </c>
+      <c r="Q2" s="4">
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2193,36 +2328,42 @@
         <v>6</v>
       </c>
       <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>22</v>
+      </c>
+      <c r="H3">
         <v>0.9</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>22</v>
       </c>
       <c r="J3">
         <v>8</v>
       </c>
+      <c r="K3">
+        <v>7</v>
+      </c>
       <c r="L3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N28" si="0">D3+F3*G3*H3</f>
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>D3+(G3*H3*F3)</f>
         <v>79.2</v>
       </c>
-      <c r="O3">
-        <f t="shared" ref="O3:O28" si="1">N3/E3</f>
+      <c r="P3">
+        <f>O3/E3</f>
         <v>13.200000000000001</v>
       </c>
-      <c r="P3" s="4">
+      <c r="Q3" s="4">
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2239,36 +2380,42 @@
         <v>6</v>
       </c>
       <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>27</v>
+      </c>
+      <c r="H4">
         <v>1</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>27</v>
       </c>
       <c r="J4">
         <v>10</v>
       </c>
+      <c r="K4">
+        <v>9</v>
+      </c>
       <c r="L4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>D4+(G4*H4*F4)</f>
         <v>135</v>
       </c>
-      <c r="O4">
-        <f t="shared" si="1"/>
+      <c r="P4">
+        <f>O4/E4</f>
         <v>22.5</v>
       </c>
-      <c r="P4" s="4">
+      <c r="Q4" s="4">
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2285,13 +2432,13 @@
         <v>5</v>
       </c>
       <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
         <v>0.3</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
       </c>
       <c r="I5">
         <v>5</v>
@@ -2309,18 +2456,21 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>D5+(G5*H5*F5)</f>
         <v>64.5</v>
       </c>
-      <c r="O5">
-        <f t="shared" si="1"/>
+      <c r="P5">
+        <f>O5/E5</f>
         <v>12.9</v>
       </c>
-      <c r="P5" s="4">
+      <c r="Q5" s="4">
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2331,19 +2481,19 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
         <v>0.5</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
       </c>
       <c r="I6">
         <v>10</v>
@@ -2361,18 +2511,21 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <f t="shared" si="0"/>
-        <v>87.5</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <f t="shared" si="1"/>
-        <v>21.875</v>
-      </c>
-      <c r="P6" s="4">
+        <f>D6+(G6*H6*F6)</f>
+        <v>82.5</v>
+      </c>
+      <c r="P6">
+        <f>O6/E6</f>
+        <v>20.625</v>
+      </c>
+      <c r="Q6" s="4">
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2383,19 +2536,19 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E7">
         <v>4</v>
       </c>
       <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
         <v>0.5</v>
-      </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-      <c r="H7">
-        <v>5</v>
       </c>
       <c r="I7">
         <v>15</v>
@@ -2413,18 +2566,21 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <f t="shared" si="0"/>
-        <v>127.5</v>
+        <v>0</v>
       </c>
       <c r="O7">
-        <f t="shared" si="1"/>
-        <v>31.875</v>
-      </c>
-      <c r="P7" s="4">
+        <f>D7+(G7*H7*F7)</f>
+        <v>117.5</v>
+      </c>
+      <c r="P7">
+        <f>O7/E7</f>
+        <v>29.375</v>
+      </c>
+      <c r="Q7" s="4">
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -2435,42 +2591,48 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <v>6</v>
       </c>
       <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
         <v>0.8</v>
       </c>
-      <c r="G8">
-        <v>4</v>
-      </c>
-      <c r="H8">
-        <v>25</v>
-      </c>
       <c r="J8">
         <v>0</v>
       </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
       <c r="L8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <f t="shared" si="0"/>
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="O8">
-        <f t="shared" si="1"/>
-        <v>13.333333333333334</v>
-      </c>
-      <c r="P8" s="4">
+        <f t="shared" ref="O8:O10" si="0">(D8*N8*L8)+(G8*H8*F8)</f>
+        <v>62</v>
+      </c>
+      <c r="P8">
+        <f>O8/E8</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q8" s="4">
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2481,42 +2643,48 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E9">
         <v>6</v>
       </c>
       <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
         <v>1</v>
       </c>
-      <c r="G9">
-        <v>4</v>
-      </c>
-      <c r="H9">
-        <v>30</v>
-      </c>
       <c r="J9">
         <v>0</v>
       </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
       <c r="L9">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
         <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="P9" s="4">
+        <v>105</v>
+      </c>
+      <c r="P9">
+        <f>O9/E9</f>
+        <v>17.5</v>
+      </c>
+      <c r="Q9" s="4">
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -2527,42 +2695,48 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E10">
         <v>6</v>
       </c>
       <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="H10">
         <v>1</v>
       </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <v>35</v>
-      </c>
       <c r="J10">
         <v>0</v>
       </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
       <c r="L10">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
         <f t="shared" si="0"/>
-        <v>175</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="1"/>
-        <v>29.166666666666668</v>
-      </c>
-      <c r="P10" s="4">
+        <v>160</v>
+      </c>
+      <c r="P10">
+        <f>O10/E10</f>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="Q10" s="4">
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -2572,19 +2746,49 @@
       <c r="C11">
         <v>1</v>
       </c>
+      <c r="D11">
+        <v>30</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0.3</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>8</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
       <c r="N11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O11" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P11" s="4">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>(D11)+(G11*H11*F11)</f>
+        <v>30</v>
+      </c>
+      <c r="P11">
+        <f>O11/E11</f>
+        <v>5</v>
+      </c>
+      <c r="Q11" s="4">
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -2594,19 +2798,49 @@
       <c r="C12">
         <v>2</v>
       </c>
+      <c r="D12">
+        <v>50</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0.5</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
       <c r="N12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O12" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P12" s="4">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>(D12)+(G12*H12*F12)</f>
+        <v>50</v>
+      </c>
+      <c r="P12">
+        <f>O12/E12</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="Q12" s="4">
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -2616,19 +2850,49 @@
       <c r="C13">
         <v>3</v>
       </c>
+      <c r="D13">
+        <v>80</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0.5</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>12</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
       <c r="N13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O13" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P13" s="4">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>(D13)+(G13*H13*F13)</f>
+        <v>80</v>
+      </c>
+      <c r="P13">
+        <f>O13/E13</f>
+        <v>16</v>
+      </c>
+      <c r="Q13" s="4">
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -2638,19 +2902,52 @@
       <c r="C14">
         <v>1</v>
       </c>
+      <c r="D14">
+        <v>60</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0.3</v>
+      </c>
+      <c r="I14">
+        <v>20</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>8</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
       <c r="N14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O14" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P14" s="4">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>(D14)+(G14*H14*F14)</f>
+        <v>60</v>
+      </c>
+      <c r="P14">
+        <f>O14/E14</f>
+        <v>6</v>
+      </c>
+      <c r="Q14" s="4">
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -2660,19 +2957,52 @@
       <c r="C15">
         <v>2</v>
       </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15">
+        <v>9</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0.5</v>
+      </c>
+      <c r="I15">
+        <v>20</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>10</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
       <c r="N15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O15" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P15" s="4">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>(D15)+(G15*H15*F15)</f>
+        <v>100</v>
+      </c>
+      <c r="P15">
+        <f>O15/E15</f>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="Q15" s="4">
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -2682,19 +3012,52 @@
       <c r="C16">
         <v>3</v>
       </c>
+      <c r="D16">
+        <v>160</v>
+      </c>
+      <c r="E16">
+        <v>9</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0.5</v>
+      </c>
+      <c r="I16">
+        <v>20</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>12</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
       <c r="N16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O16" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P16" s="4">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f>(D16)+(G16*H16*F16)</f>
+        <v>160</v>
+      </c>
+      <c r="P16">
+        <f>O16/E16</f>
+        <v>17.777777777777779</v>
+      </c>
+      <c r="Q16" s="4">
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -2704,19 +3067,52 @@
       <c r="C17">
         <v>1</v>
       </c>
+      <c r="D17">
+        <v>18</v>
+      </c>
+      <c r="E17" s="7">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0.3</v>
+      </c>
+      <c r="I17">
+        <v>15</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17" s="7">
+        <v>5</v>
+      </c>
+      <c r="L17" s="7">
+        <v>8</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
       <c r="N17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O17" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P17" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="O17">
+        <f>(D17*N17*L17)+(G17*H17*F17)</f>
+        <v>72</v>
+      </c>
+      <c r="P17">
+        <f>O17/E17</f>
+        <v>9</v>
+      </c>
+      <c r="Q17" s="4">
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -2726,19 +3122,52 @@
       <c r="C18">
         <v>2</v>
       </c>
+      <c r="D18">
+        <v>20</v>
+      </c>
+      <c r="E18" s="7">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0.5</v>
+      </c>
+      <c r="I18">
+        <v>15</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18" s="7">
+        <v>7</v>
+      </c>
+      <c r="L18" s="7">
+        <v>10</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
       <c r="N18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O18" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P18" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="O18">
+        <f>(D18*N18*L18)+(G18*H18*F18)</f>
+        <v>100</v>
+      </c>
+      <c r="P18">
+        <f>O18/E18</f>
+        <v>14.285714285714286</v>
+      </c>
+      <c r="Q18" s="4">
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -2748,19 +3177,52 @@
       <c r="C19">
         <v>3</v>
       </c>
+      <c r="D19">
+        <v>30</v>
+      </c>
+      <c r="E19" s="7">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0.5</v>
+      </c>
+      <c r="I19">
+        <v>15</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19" s="7">
+        <v>9</v>
+      </c>
+      <c r="L19" s="7">
+        <v>12</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
       <c r="N19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O19" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P19" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="O19">
+        <f>(D19*N19*L19)+(G19*H19*F19)</f>
+        <v>180</v>
+      </c>
+      <c r="P19">
+        <f>O19/E19</f>
+        <v>25.714285714285715</v>
+      </c>
+      <c r="Q19" s="4">
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -2770,19 +3232,52 @@
       <c r="C20">
         <v>1</v>
       </c>
+      <c r="D20">
+        <v>55</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>1.2</v>
+      </c>
+      <c r="H20">
+        <v>0.3</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0.1</v>
+      </c>
+      <c r="M20">
+        <v>5</v>
+      </c>
       <c r="N20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O20" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P20" s="4">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f>D20+(G20*H20*F20)</f>
+        <v>56.08</v>
+      </c>
+      <c r="P20">
+        <f>O20/E20</f>
+        <v>11.215999999999999</v>
+      </c>
+      <c r="Q20" s="4">
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -2792,19 +3287,52 @@
       <c r="C21">
         <v>2</v>
       </c>
+      <c r="D21">
+        <v>70</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>1.5</v>
+      </c>
+      <c r="H21">
+        <v>0.5</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0.1</v>
+      </c>
+      <c r="M21">
+        <v>5</v>
+      </c>
       <c r="N21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O21" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P21" s="4">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <f>D21+(G21*H21*F21)</f>
+        <v>72.25</v>
+      </c>
+      <c r="P21">
+        <f>O21/E21</f>
+        <v>18.0625</v>
+      </c>
+      <c r="Q21" s="4">
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2814,19 +3342,52 @@
       <c r="C22">
         <v>3</v>
       </c>
+      <c r="D22">
+        <v>120</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>1.7</v>
+      </c>
+      <c r="H22">
+        <v>0.5</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0.1</v>
+      </c>
+      <c r="M22">
+        <v>5</v>
+      </c>
       <c r="N22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O22" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P22" s="4">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f>D22+(G22*H22*F22)</f>
+        <v>122.55</v>
+      </c>
+      <c r="P22">
+        <f>O22/E22</f>
+        <v>30.637499999999999</v>
+      </c>
+      <c r="Q22" s="4">
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -2836,19 +3397,52 @@
       <c r="C23">
         <v>1</v>
       </c>
+      <c r="D23">
+        <v>22</v>
+      </c>
+      <c r="E23" s="6">
+        <v>8</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>1.2</v>
+      </c>
+      <c r="H23">
+        <v>0.3</v>
+      </c>
+      <c r="I23">
+        <v>15</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23" s="6">
+        <v>8</v>
+      </c>
+      <c r="M23">
+        <v>10</v>
+      </c>
       <c r="N23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O23" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P23" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="O23">
+        <f>(D23*N23*L23)+(G23*H23*F23)</f>
+        <v>89.08</v>
+      </c>
+      <c r="P23">
+        <f>O23/E23</f>
+        <v>11.135</v>
+      </c>
+      <c r="Q23" s="4">
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -2858,19 +3452,52 @@
       <c r="C24">
         <v>2</v>
       </c>
+      <c r="D24">
+        <v>25</v>
+      </c>
+      <c r="E24" s="6">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>1.5</v>
+      </c>
+      <c r="H24">
+        <v>0.5</v>
+      </c>
+      <c r="I24">
+        <v>15</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24" s="6">
+        <v>10</v>
+      </c>
+      <c r="M24">
+        <v>10</v>
+      </c>
       <c r="N24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O24" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P24" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="O24">
+        <f>(D24*N24*L24)+(G24*H24*F24)</f>
+        <v>128</v>
+      </c>
+      <c r="P24">
+        <f>O24/E24</f>
+        <v>18.285714285714285</v>
+      </c>
+      <c r="Q24" s="4">
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -2880,19 +3507,52 @@
       <c r="C25">
         <v>3</v>
       </c>
+      <c r="D25">
+        <v>35</v>
+      </c>
+      <c r="E25" s="6">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>1.7</v>
+      </c>
+      <c r="H25">
+        <v>0.5</v>
+      </c>
+      <c r="I25">
+        <v>15</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25" s="6">
+        <v>12</v>
+      </c>
+      <c r="M25">
+        <v>10</v>
+      </c>
       <c r="N25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O25" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P25" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="O25">
+        <f>(D25*N25*L25)+(G25*H25*F25)</f>
+        <v>213.4</v>
+      </c>
+      <c r="P25">
+        <f>O25/E25</f>
+        <v>30.485714285714288</v>
+      </c>
+      <c r="Q25" s="4">
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -2902,19 +3562,52 @@
       <c r="C26">
         <v>1</v>
       </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>4</v>
+      </c>
+      <c r="G26">
+        <v>1.5</v>
+      </c>
+      <c r="H26">
+        <v>0.5</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0.2</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
       <c r="N26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O26" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P26" s="4">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <f>D26+(G26*H26*F26)</f>
+        <v>3</v>
+      </c>
+      <c r="P26">
+        <f>O26/E26</f>
+        <v>0.75</v>
+      </c>
+      <c r="Q26" s="4">
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -2924,19 +3617,52 @@
       <c r="C27">
         <v>2</v>
       </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>5</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>0.7</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0.2</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
       <c r="N27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O27" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P27" s="4">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <f>D27+(G27*H27*F27)</f>
+        <v>7</v>
+      </c>
+      <c r="P27">
+        <f>O27/E27</f>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="Q27" s="4">
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -2946,19 +3672,53 @@
       <c r="C28">
         <v>3</v>
       </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>6</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0.2</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
       <c r="N28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O28" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P28" s="4">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f>D28+(G28*H28*F28)</f>
+        <v>12</v>
+      </c>
+      <c r="P28">
+        <f>O28/E28</f>
+        <v>4</v>
+      </c>
+      <c r="Q28" s="4">
         <v>26.888888888888889</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q28" xr:uid="{30F44E55-3490-4989-BF47-DCCD22AFF76E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Spells check, Thunder Ultimate, and start of boss
</commit_message>
<xml_diff>
--- a/Assets/Systems.xlsx
+++ b/Assets/Systems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project_Witch_Hunt\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44994C57-84F7-4DBD-B343-AA36E21AEA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEADA1A-6500-4DC8-A339-43DC05435E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{532FCD95-2C2A-4B56-85A4-F5F3E8F1C2DC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{532FCD95-2C2A-4B56-85A4-F5F3E8F1C2DC}"/>
   </bookViews>
   <sheets>
     <sheet name="CharacterStats" sheetId="3" r:id="rId1"/>
@@ -20,6 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BaseSpellsStats!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Dictionary!$A$1:$F$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">SpecialSpellsStats!$A$1:$Q$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="94">
   <si>
     <t>Base Spells</t>
   </si>
@@ -165,33 +166,9 @@
     <t>Special</t>
   </si>
   <si>
-    <t>Fire attack in an angle, this angle can increase or decrease depending on the tier of the spell, the range should also change. Like a shotgun</t>
-  </si>
-  <si>
-    <t>A fire ring that revolves around the player, burning nearby enemies and also healing the player a little.</t>
-  </si>
-  <si>
-    <t>A line spell of fire in a certain direction, cast from the ground.</t>
-  </si>
-  <si>
-    <t>A sphere of frost that pushes enemies away. a sphere that is cast from the player outward, or an ice sphere explosion from the player.</t>
-  </si>
-  <si>
-    <t>Ice spikes that comes from the floor to hit enemies, in a round radius.</t>
-  </si>
-  <si>
-    <t>sequential shots of ice shards for a certain duration.</t>
-  </si>
-  <si>
-    <t>A totem of lightning is cast to the aim position casting lightning attacks</t>
-  </si>
-  <si>
     <t>A ball of lightning that keeps moving around the player dealing damage to enemeis.</t>
   </si>
   <si>
-    <t>A constant line of lightning that is cast forward.</t>
-  </si>
-  <si>
     <t>Base</t>
   </si>
   <si>
@@ -292,6 +269,63 @@
   </si>
   <si>
     <t>StatusEffect Dmg</t>
+  </si>
+  <si>
+    <t>Working?</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Special Effects</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Ultimate</t>
+  </si>
+  <si>
+    <t>FireMeteor</t>
+  </si>
+  <si>
+    <t>Thunder</t>
+  </si>
+  <si>
+    <t>Blizzard</t>
+  </si>
+  <si>
+    <t>Y, BUT NOT GOOD</t>
+  </si>
+  <si>
+    <t>A fire ring that revolves around the caster, burning nearby enemies and healing the caster</t>
+  </si>
+  <si>
+    <t>A fire attack in an angle, affecting every enemy with a certain angle of attack from the caster</t>
+  </si>
+  <si>
+    <t>A trail of fire in a certain direction, cast from the ground, burning enemies that come close to it</t>
+  </si>
+  <si>
+    <t>A beam of lightning cast in a straight line hitting all enemies that touch it.</t>
+  </si>
+  <si>
+    <t>A totem that casts lightning spells to enemies that come close to it.</t>
+  </si>
+  <si>
+    <t>Ice spikes that grow from the floor to hit enemies</t>
+  </si>
+  <si>
+    <t>Sequential shots of ice shards for a certain duration</t>
+  </si>
+  <si>
+    <t>A sphere of frost that pushes enemies away</t>
+  </si>
+  <si>
+    <t>A meteor of fire cast from the sky that falls into enemies.</t>
+  </si>
+  <si>
+    <t>A blizzard cast with the caster that hits every enemy on its path</t>
   </si>
 </sst>
 </file>
@@ -699,26 +733,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A50200A-D5C9-4036-ACBE-BAEB92E92EFD}">
   <dimension ref="A2:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>29</v>
       </c>
@@ -726,10 +760,10 @@
         <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -759,10 +793,10 @@
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="W3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -818,7 +852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -885,7 +919,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -952,7 +986,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1014,7 +1048,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1062,7 +1096,7 @@
         <v>16.666666666666668</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1094,7 +1128,7 @@
         <v>26.666666666666668</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1126,12 +1160,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
         <v>32</v>
@@ -1150,12 +1184,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -1177,12 +1211,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -1194,12 +1228,12 @@
         <v>2363</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -1218,12 +1252,12 @@
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -1243,12 +1277,12 @@
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -1268,12 +1302,12 @@
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -1283,12 +1317,12 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
         <v>32</v>
@@ -1297,7 +1331,7 @@
         <v>0</v>
       </c>
       <c r="U18" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="V18" t="s">
         <v>6</v>
@@ -1307,12 +1341,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
@@ -1325,7 +1359,7 @@
         <v>515</v>
       </c>
       <c r="U19" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="V19" t="s">
         <v>7</v>
@@ -1335,12 +1369,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -1353,7 +1387,7 @@
         <v>1125</v>
       </c>
       <c r="U20" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="V20" t="s">
         <v>8</v>
@@ -1363,12 +1397,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -1381,7 +1415,7 @@
         <v>2534</v>
       </c>
       <c r="U21" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="V21" t="s">
         <v>6</v>
@@ -1390,9 +1424,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="U22" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="V22" t="s">
         <v>7</v>
@@ -1401,9 +1435,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="U23" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="V23" t="s">
         <v>8</v>
@@ -1412,7 +1446,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V25" t="s">
         <v>6</v>
       </c>
@@ -1421,7 +1455,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V26" t="s">
         <v>7</v>
       </c>
@@ -1430,7 +1464,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V27" t="s">
         <v>8</v>
       </c>
@@ -1439,14 +1473,14 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B34" t="s">
         <v>28</v>
@@ -1462,9 +1496,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
         <v>28</v>
@@ -1484,9 +1518,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
         <v>28</v>
@@ -1506,9 +1540,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B37" t="s">
         <v>28</v>
@@ -1523,9 +1557,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B38" t="s">
         <v>28</v>
@@ -1541,9 +1575,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B39" t="s">
         <v>28</v>
@@ -1559,30 +1593,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C42" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D42" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="G42" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="H42" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I42" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="J42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -1616,7 +1650,7 @@
         <v>8.5714285714285712</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -1650,7 +1684,7 @@
         <v>18.743801652892561</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -1701,20 +1735,20 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1734,7 +1768,7 @@
         <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="H1" t="s">
         <v>12</v>
@@ -1743,13 +1777,13 @@
         <v>25</v>
       </c>
       <c r="J1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="K1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1786,7 +1820,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1823,7 +1857,7 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1860,7 +1894,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1894,7 +1928,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1928,7 +1962,7 @@
         <v>16.666666666666668</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1962,7 +1996,7 @@
         <v>26.666666666666668</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1996,7 +2030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -2030,7 +2064,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -2064,7 +2098,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2085,7 +2119,7 @@
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2106,7 +2140,7 @@
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2192,28 +2226,28 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" customWidth="1"/>
-    <col min="17" max="17" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2233,7 +2267,7 @@
         <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="H1" t="s">
         <v>12</v>
@@ -2242,31 +2276,31 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="K1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="L1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="M1" t="s">
         <v>4</v>
       </c>
       <c r="N1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="O1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="P1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="Q1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2318,7 +2352,7 @@
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2370,7 +2404,7 @@
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2422,7 +2456,7 @@
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2477,7 +2511,7 @@
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2532,7 +2566,7 @@
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2587,7 +2621,7 @@
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -2639,7 +2673,7 @@
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2691,7 +2725,7 @@
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -2743,7 +2777,7 @@
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -2795,7 +2829,7 @@
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -2847,7 +2881,7 @@
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -2899,7 +2933,7 @@
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -2954,7 +2988,7 @@
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -3009,7 +3043,7 @@
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -3064,7 +3098,7 @@
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -3119,7 +3153,7 @@
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -3174,7 +3208,7 @@
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -3229,7 +3263,7 @@
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -3284,7 +3318,7 @@
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -3339,7 +3373,7 @@
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -3394,7 +3428,7 @@
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -3449,7 +3483,7 @@
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -3504,7 +3538,7 @@
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -3559,7 +3593,7 @@
         <v>26.888888888888889</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -3614,7 +3648,7 @@
         <v>10.666666666666666</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -3669,7 +3703,7 @@
         <v>16.888888888888889</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -3732,19 +3766,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0B8A037-056C-4A36-B3A6-CFAFCD5D282E}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="125.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="125.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -3757,50 +3792,74 @@
       <c r="D1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -3811,10 +3870,16 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="E5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -3825,10 +3890,16 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="E6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -3839,10 +3910,16 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="E7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -3853,10 +3930,16 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -3867,10 +3950,16 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+      <c r="E9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -3881,10 +3970,16 @@
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="E10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -3895,10 +3990,16 @@
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+      <c r="E11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -3909,10 +4010,16 @@
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="E12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -3923,10 +4030,71 @@
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>91</v>
+      </c>
+      <c r="E13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F16" xr:uid="{A0B8A037-056C-4A36-B3A6-CFAFCD5D282E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>